<commit_message>
draw functions and map
</commit_message>
<xml_diff>
--- a/venv/Rockgame/config.xlsx
+++ b/venv/Rockgame/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Level" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,10 +33,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>enemy_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>player_position</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -135,6 +131,19 @@
   <si>
     <t>敌人最大数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>10,12</t>
+  </si>
+  <si>
+    <t>10,13</t>
   </si>
 </sst>
 </file>
@@ -493,7 +502,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
@@ -531,24 +540,24 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -565,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -576,40 +585,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -626,7 +633,58 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -639,9 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -655,30 +711,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -686,22 +742,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -709,19 +765,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
       </c>
       <c r="G4">
         <v>1</v>

</xml_diff>